<commit_message>
supplier in add_item_second is not required
</commit_message>
<xml_diff>
--- a/Inventory Report.xlsx
+++ b/Inventory Report.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
-  <si>
-    <t>CENTRAL NEGROS POWER RELIABILITY, INC.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
+  <si>
+    <t>PROGEN DIESEL TECH</t>
   </si>
   <si>
     <t>MATERIAL INVENTORY REPORT</t>
@@ -35,7 +35,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2019-03-01 - 2019-03-28</t>
+    <t>2019-03-01 - 2019-04-08</t>
   </si>
   <si>
     <t>Warehouse</t>
@@ -44,9 +44,15 @@
     <t>Main Category</t>
   </si>
   <si>
+    <t>Engine and Auxiliary Parts and Accessories</t>
+  </si>
+  <si>
     <t>Sub-Category</t>
   </si>
   <si>
+    <t>Engine/Mechanical (Pielstick)</t>
+  </si>
+  <si>
     <t>No.</t>
   </si>
   <si>
@@ -57,6 +63,216 @@
   </si>
   <si>
     <t>Avail. Qty</t>
+  </si>
+  <si>
+    <t>059Q014</t>
+  </si>
+  <si>
+    <t>Shaft/Spindle PF 59-14</t>
+  </si>
+  <si>
+    <t>075Q091</t>
+  </si>
+  <si>
+    <t>O-ring 001/00325-0070 PF 75-91</t>
+  </si>
+  <si>
+    <t>032Q051</t>
+  </si>
+  <si>
+    <t>Plug PF 32-51</t>
+  </si>
+  <si>
+    <t>022Q007</t>
+  </si>
+  <si>
+    <t>Washer PF 22-7</t>
+  </si>
+  <si>
+    <t>032Q117</t>
+  </si>
+  <si>
+    <t>Tapered Pin, PN 250032011700 (NKK) stainless PF 32-117A</t>
+  </si>
+  <si>
+    <t>Tapered Pin, PN 250032011700 (NKK) ordinary PF 32-117B</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Locking Piece, GR32, PN140, (L-Washer) PF 32-140</t>
+  </si>
+  <si>
+    <t>00.225.05.026.5</t>
+  </si>
+  <si>
+    <t>Pin 001/00230-0390 PF 54-117</t>
+  </si>
+  <si>
+    <t>017Q216</t>
+  </si>
+  <si>
+    <t>Spacing Washer PF 17-216</t>
+  </si>
+  <si>
+    <t>019Q007</t>
+  </si>
+  <si>
+    <t>Valve/Needle Valve PF 19-7</t>
+  </si>
+  <si>
+    <t>020Q013</t>
+  </si>
+  <si>
+    <t>Slotted Set Screw PF 20-13</t>
+  </si>
+  <si>
+    <t>00.157.001600</t>
+  </si>
+  <si>
+    <t>Copper Packing PF 60-14</t>
+  </si>
+  <si>
+    <t>016Q006</t>
+  </si>
+  <si>
+    <t>Packing / Special Joint, PN 312329300  PF 16-6</t>
+  </si>
+  <si>
+    <t>019Q006</t>
+  </si>
+  <si>
+    <t>Valve Rod (Valve Stem) PF 19-6A</t>
+  </si>
+  <si>
+    <t>Valve Rod (Valve Stem) PF 19-6B</t>
+  </si>
+  <si>
+    <t>00.001.10.010.5</t>
+  </si>
+  <si>
+    <t>Bolt 001/00230 PF 54-32</t>
+  </si>
+  <si>
+    <t>02.054.0112.00</t>
+  </si>
+  <si>
+    <t>Push Rod 001/00230-0380 PF 54-112</t>
+  </si>
+  <si>
+    <t>103Q035</t>
+  </si>
+  <si>
+    <t>Packing / Felt Packing PF 103-35</t>
+  </si>
+  <si>
+    <t>103Q037</t>
+  </si>
+  <si>
+    <t>Packing / Felt Packing PF 103-37</t>
+  </si>
+  <si>
+    <t>136Q421</t>
+  </si>
+  <si>
+    <t>Bolt PF 136-421</t>
+  </si>
+  <si>
+    <t>142Q280</t>
+  </si>
+  <si>
+    <t>Hexagonal Socket Head Screw/ Socket Head Bolt PF 142-280</t>
+  </si>
+  <si>
+    <t>030Q018</t>
+  </si>
+  <si>
+    <t>Upper Spring Collar PF 30-18</t>
+  </si>
+  <si>
+    <t>096Q005</t>
+  </si>
+  <si>
+    <t>Lubrication Piece/Oil Intake Pin PF 96-5</t>
+  </si>
+  <si>
+    <t>096Q014</t>
+  </si>
+  <si>
+    <t>Tongued Washer PF 96-14</t>
+  </si>
+  <si>
+    <t>096Q317</t>
+  </si>
+  <si>
+    <t>Tongued Washer PF 96-317</t>
+  </si>
+  <si>
+    <t>102Q067</t>
+  </si>
+  <si>
+    <t>Connection Piece PF 102-67</t>
+  </si>
+  <si>
+    <t>102Q205</t>
+  </si>
+  <si>
+    <t>Bolt PF 102-205</t>
+  </si>
+  <si>
+    <t>102Q214</t>
+  </si>
+  <si>
+    <t>Circlip PF 102-214</t>
+  </si>
+  <si>
+    <t>102Q308</t>
+  </si>
+  <si>
+    <t>Shaft PF 102-308</t>
+  </si>
+  <si>
+    <t>102Q052</t>
+  </si>
+  <si>
+    <t>Pin PF 102-52</t>
+  </si>
+  <si>
+    <t>102Q056</t>
+  </si>
+  <si>
+    <t>Bush (Copper) PF 102-56</t>
+  </si>
+  <si>
+    <t>102Q087</t>
+  </si>
+  <si>
+    <t>Nut (Lock) PF 102-87</t>
+  </si>
+  <si>
+    <t>102Q118</t>
+  </si>
+  <si>
+    <t>Dowel Pin / Linkage Pin PF 102-118</t>
+  </si>
+  <si>
+    <t>PF 102-84</t>
+  </si>
+  <si>
+    <t>Split Pin PF 102-84</t>
+  </si>
+  <si>
+    <t>102Q089</t>
+  </si>
+  <si>
+    <t>Split Pin PF 102-89</t>
+  </si>
+  <si>
+    <t>125Q050</t>
+  </si>
+  <si>
+    <t>Self Lock Nut PF 125-50</t>
   </si>
   <si>
     <t>005Q022</t>
@@ -538,7 +754,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I2" sqref="I2"/>
@@ -609,27 +825,31 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -637,7 +857,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -646,45 +866,978 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="2">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="2">
+        <v>7</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="2">
+        <v>9</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="2">
+        <v>34</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="2">
+        <v>58</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="3">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2">
+        <v>40</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="3">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="3">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="2">
+        <v>46</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="3">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="2">
+        <v>21</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="3">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="2">
+        <v>30</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="3">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="2">
+        <v>45</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="3">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="2">
+        <v>47</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="3">
+        <v>14</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="2">
+        <v>32</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="3">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="2">
+        <v>13</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="3">
+        <v>16</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="2">
+        <v>4</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="3">
+        <v>17</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="2">
+        <v>8</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="3">
+        <v>18</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="2">
+        <v>25</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="3">
+        <v>19</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="2">
+        <v>26</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="3">
+        <v>20</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="2">
+        <v>14</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="3">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="2">
+        <v>20</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="3">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="2">
+        <v>3</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="3">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="2">
+        <v>6</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="3">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="2">
+        <v>11</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="3">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="2">
+        <v>54</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="3">
+        <v>26</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="2">
+        <v>8</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="3">
+        <v>27</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="3">
+        <v>28</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="2">
+        <v>31</v>
+      </c>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="3">
+        <v>29</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="2">
+        <v>1</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="3">
+        <v>30</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="2">
+        <v>21</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="3">
+        <v>31</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="2">
+        <v>77</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="3">
+        <v>32</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="2">
+        <v>48</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="3">
+        <v>33</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="2">
+        <v>30</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="3">
+        <v>34</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="2">
+        <v>63</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="3">
+        <v>35</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="2">
+        <v>74</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="3">
+        <v>36</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="2">
+        <v>12</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="3">
+        <v>37</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="2">
+        <v>16</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
-    <protectedRange name="p3a2774e87537806651c7c974f8588f09" sqref="A11:L11" password="C724"/>
+    <protectedRange name="pc7fee7a9cd7600357aabcbcc1bf4b445" sqref="A11:H11" password="C724"/>
+    <protectedRange name="p92880f929fe609d4207311c6392005e7" sqref="A12:H12" password="C724"/>
+    <protectedRange name="p539771250c163552e62a21739a7b35c5" sqref="A13:H13" password="C724"/>
+    <protectedRange name="p9f5d7d6e0c660701d7077c653c593bc3" sqref="A14:H14" password="C724"/>
+    <protectedRange name="p39b3a4ebd78e21886795a253f3bf93e1" sqref="A15:H15" password="C724"/>
+    <protectedRange name="pdd56e45bebd4b23600ce1b3814655254" sqref="A16:H16" password="C724"/>
+    <protectedRange name="p4351fd45f124ad1ea7153b2a53e1b2b6" sqref="A17:H17" password="C724"/>
+    <protectedRange name="pb159d50ff7fb9ab27d303cad23f41f8d" sqref="A18:H18" password="C724"/>
+    <protectedRange name="p02b38ae7131dd4ee9221b6c1e303f3d9" sqref="A19:H19" password="C724"/>
+    <protectedRange name="p01a6de3afac7e96409654dd595ba068b" sqref="A20:H20" password="C724"/>
+    <protectedRange name="p6a641f3e9c850988517f5f784c6039e8" sqref="A21:H21" password="C724"/>
+    <protectedRange name="p6a357b76a4abd122aa966308510fb171" sqref="A22:H22" password="C724"/>
+    <protectedRange name="p17b76adfc0de5a0998754277bcc8d8d0" sqref="A23:H23" password="C724"/>
+    <protectedRange name="pb50081fbf3c93aa584956db925927cb5" sqref="A24:H24" password="C724"/>
+    <protectedRange name="pdb0acdd8cde75aa3b3e3292232373d90" sqref="A25:H25" password="C724"/>
+    <protectedRange name="pba8d36e62f0a76836998a860aba15a58" sqref="A26:H26" password="C724"/>
+    <protectedRange name="p01ec34752847c49b6571f28204e8781c" sqref="A27:H27" password="C724"/>
+    <protectedRange name="p54a4d7acfef3d6399a79db59db3e0a2c" sqref="A28:H28" password="C724"/>
+    <protectedRange name="p55cfcc81cc89432a8e2cf22270cc9141" sqref="A29:H29" password="C724"/>
+    <protectedRange name="p90fa6a027ac8ebbe0c4d8af6e4cdf6ec" sqref="A30:H30" password="C724"/>
+    <protectedRange name="pab270de58a107cf8b9ef9365f1ea388e" sqref="A31:H31" password="C724"/>
+    <protectedRange name="pea2b665f124f246aa9ed77ae22f2687b" sqref="A32:H32" password="C724"/>
+    <protectedRange name="p9643bd2bf5a8d71d1930f86da09c3cff" sqref="A33:H33" password="C724"/>
+    <protectedRange name="p402ab31fe6f4ae21cbd310e2ae0c55f3" sqref="A34:H34" password="C724"/>
+    <protectedRange name="p7abd0adc40976882aa8fbe024ea8b221" sqref="A35:H35" password="C724"/>
+    <protectedRange name="p2fbf9e6da57821468b4f051a57eeb77b" sqref="A36:H36" password="C724"/>
+    <protectedRange name="p2e790247cea7f6afbd1a7f5bb3b28e06" sqref="A37:H37" password="C724"/>
+    <protectedRange name="pb896b4356f41dcb5d85cf91132727d41" sqref="A38:H38" password="C724"/>
+    <protectedRange name="pd1b4985a71e9d989ee97a2a1083b3a4c" sqref="A39:H39" password="C724"/>
+    <protectedRange name="p6bd3100b516a16e16a853eeb46bd8870" sqref="A40:H40" password="C724"/>
+    <protectedRange name="p0f417cb9da397245fce8cf52cb2d15d2" sqref="A41:H41" password="C724"/>
+    <protectedRange name="p092efa2e1e41ebd31d22c4feaab698d7" sqref="A42:H42" password="C724"/>
+    <protectedRange name="p9f21f9e46d95319f33df2256818f3ee8" sqref="A43:H43" password="C724"/>
+    <protectedRange name="p296b7171c585bd63b43420e6dd30e8d7" sqref="A44:H44" password="C724"/>
+    <protectedRange name="pe04252d00a532cf426a56d541c383f81" sqref="A45:H45" password="C724"/>
+    <protectedRange name="pdd3e4fc3b1803d5d684a38bbfcbd1029" sqref="A46:H46" password="C724"/>
+    <protectedRange name="p6bc49966b7a791663fbb53f6f0bf01be" sqref="A47:H47" password="C724"/>
   </protectedRanges>
   <mergeCells>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:K48"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:J10"/>
     <mergeCell ref="K10:L10"/>

</xml_diff>

<commit_message>
changes forget to commit
</commit_message>
<xml_diff>
--- a/Inventory Report.xlsx
+++ b/Inventory Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="142">
   <si>
     <t>PROGEN DIESEL TECH</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Purok San Jose, Brgy. Calumangan, Bago City</t>
   </si>
   <si>
-    <t>TO DATE</t>
+    <t>AS OF November 26, 2019</t>
   </si>
   <si>
     <t>Tel. No. 476 - 7382</t>
@@ -35,7 +35,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2019-05-01 - 2019-08-06</t>
+    <t>2019-07-01 - 2019-11-26</t>
   </si>
   <si>
     <t>Warehouse</t>
@@ -59,34 +59,376 @@
     <t>Avail. Qty</t>
   </si>
   <si>
+    <t>CON-CHE_1004</t>
+  </si>
+  <si>
+    <t>Acid; Muriatic</t>
+  </si>
+  <si>
+    <t>CON-CHE_1005</t>
+  </si>
+  <si>
+    <t>Anti-Corrosion Paper, Size: 1 m x 25 m</t>
+  </si>
+  <si>
+    <t>CON-CON_1008</t>
+  </si>
+  <si>
+    <t>Blade; Hacksaw, 18 TPI</t>
+  </si>
+  <si>
+    <t>CON-CHE_1003</t>
+  </si>
+  <si>
+    <t>Blue Silica Gel, Bead Size: 4-6mm, 5 kgs./moisture barrier bag</t>
+  </si>
+  <si>
+    <t>CON-HOU_1002</t>
+  </si>
+  <si>
+    <t>Broom (Paypay)</t>
+  </si>
+  <si>
+    <t>CON-CON_1006</t>
+  </si>
+  <si>
+    <t>Brush, Paint, 4"</t>
+  </si>
+  <si>
+    <t>CON-CON_1005</t>
+  </si>
+  <si>
+    <t>Brush, Steel</t>
+  </si>
+  <si>
+    <t>PRO-PF 22-328</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>CON-FUE_1001</t>
+  </si>
+  <si>
+    <t>Diesel, Fuel-Save</t>
+  </si>
+  <si>
+    <t>CON-CON_1007</t>
+  </si>
+  <si>
+    <t>Epoxy; Primer Gray with Catalyst</t>
+  </si>
+  <si>
+    <t>PRO-PF 15-00</t>
+  </si>
+  <si>
+    <t>Gasket (O-ring), 2.5mm x 9.5mm</t>
+  </si>
+  <si>
+    <t>CON-HOU_1003</t>
+  </si>
+  <si>
+    <t>Gloves, Cotton</t>
+  </si>
+  <si>
+    <t>CON-HOU_1005</t>
+  </si>
+  <si>
+    <t>Gloves, Cotton with Rubber</t>
+  </si>
+  <si>
+    <t>PRO-PF 22-127</t>
+  </si>
+  <si>
+    <t>Joint Ring</t>
+  </si>
+  <si>
+    <t>PRO-PF 3-6</t>
+  </si>
+  <si>
+    <t>Locking Wire</t>
+  </si>
+  <si>
+    <t>CON-CON_1015</t>
+  </si>
+  <si>
+    <t>Lumber: Good, 2" x 3" x 6 ft, Mahogany</t>
+  </si>
+  <si>
+    <t>CON-CON_1013</t>
+  </si>
+  <si>
+    <t>Lumber; Good, 2" x 3" x 10 ft, Mahogany</t>
+  </si>
+  <si>
+    <t>CON-CON_1014</t>
+  </si>
+  <si>
+    <t>Lumber; Good, 2" x 3" x 8 ft, Mahogany</t>
+  </si>
+  <si>
+    <t>CON-OFF_1001</t>
+  </si>
+  <si>
+    <t>Marker, Metal, Color: Yellow</t>
+  </si>
+  <si>
+    <t>FFE-PPE_1001</t>
+  </si>
+  <si>
+    <t>Mask; Face (50 pcs.)</t>
+  </si>
+  <si>
+    <t>CON-CON_1012</t>
+  </si>
+  <si>
+    <t>Nails; Common, 1 1/2"</t>
+  </si>
+  <si>
+    <t>CON-CON_1011</t>
+  </si>
+  <si>
+    <t>Nails; Common, 2 1/2"</t>
+  </si>
+  <si>
+    <t>CON-CON_1010</t>
+  </si>
+  <si>
+    <t>Nails; Common, 3"</t>
+  </si>
+  <si>
+    <t>CON-CON_1009</t>
+  </si>
+  <si>
+    <t>Nails; Common, 4"</t>
+  </si>
+  <si>
+    <t>PRO-PF 15-29</t>
+  </si>
+  <si>
+    <t>O - ring</t>
+  </si>
+  <si>
+    <t>PRO-PF 8-5</t>
+  </si>
+  <si>
+    <t>O-ring</t>
+  </si>
+  <si>
+    <t>PRO-PF 54-136</t>
+  </si>
+  <si>
+    <t>O-ring (SEMT)</t>
+  </si>
+  <si>
+    <t>PRO-PF 20-347</t>
+  </si>
+  <si>
+    <t>O-ring (SEMT), 2mm x 9mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 54-135</t>
+  </si>
+  <si>
+    <t>O-ring (SEMT), 3.5mm x 25mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 18-58</t>
+  </si>
+  <si>
+    <t>O-ring, 2.5mm x 70mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 40-7</t>
+  </si>
+  <si>
+    <t>O-ring, 26 mm x 7 mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 1-14</t>
+  </si>
+  <si>
+    <t>O-ring, 3.5mm x 25.5mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 15-20</t>
+  </si>
+  <si>
+    <t>O-ring, 3.5mm x 30mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 5-7</t>
+  </si>
+  <si>
+    <t>O-ring, 339 mm x 5 mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 42-5</t>
+  </si>
+  <si>
+    <t>O-ring, 3mm x 41mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 42-8</t>
+  </si>
+  <si>
+    <t>O-ring, 3mm x 50mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 22-332</t>
+  </si>
+  <si>
+    <t>O-ring, 3mm x 56mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 17-111</t>
+  </si>
+  <si>
+    <t>O-ring, 3mm x 71mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 17-112</t>
+  </si>
+  <si>
+    <t>O-ring, 40.64 mm x 3.53 mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 30-6</t>
+  </si>
+  <si>
+    <t>O-ring, 59.69 mm x 5.33 mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 15-28</t>
+  </si>
+  <si>
+    <t>O-ring, 5mm x 124mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 18-59</t>
+  </si>
+  <si>
+    <t>O-ring, 5mm x 50mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 18-57</t>
+  </si>
+  <si>
+    <t>O-ring, 5mm x 52mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 20-335</t>
+  </si>
+  <si>
+    <t>O-ring, 5mm x 80mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 1-15</t>
+  </si>
+  <si>
+    <t>O-ring, 5mm x 93mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 75-210</t>
+  </si>
+  <si>
+    <t>O-ring, 7mm x 176mm</t>
+  </si>
+  <si>
+    <t>PRO-PF 82-8</t>
+  </si>
+  <si>
+    <t>Oil Seal, 64 x 80 x 13</t>
+  </si>
+  <si>
+    <t>PRO-PF 65-317</t>
+  </si>
+  <si>
+    <t>Oring</t>
+  </si>
+  <si>
+    <t>CON-CON_1002</t>
+  </si>
+  <si>
+    <t>Paint Brush 1"</t>
+  </si>
+  <si>
+    <t>CON-CON_1004</t>
+  </si>
+  <si>
+    <t>Paint Brush 2"</t>
+  </si>
+  <si>
+    <t>CON-FUE_1002</t>
+  </si>
+  <si>
+    <t>Penetrating Oil Multi Use, WD40</t>
+  </si>
+  <si>
+    <t>CON-HOU_1001</t>
+  </si>
+  <si>
+    <t>Rags, Cotton</t>
+  </si>
+  <si>
+    <t>CON-CHE_1002</t>
+  </si>
+  <si>
+    <t>Rust Converter</t>
+  </si>
+  <si>
+    <t>CON-CON_1003</t>
+  </si>
+  <si>
+    <t>Sand Paper, G120</t>
+  </si>
+  <si>
     <t>CON-CON_1001</t>
   </si>
   <si>
     <t>Scraper, Industrial; Size: 2"</t>
   </si>
   <si>
-    <t>CON-FUE_1002</t>
-  </si>
-  <si>
-    <t>Penetrating Oil Multi Use, WD40</t>
-  </si>
-  <si>
-    <t>_1001</t>
-  </si>
-  <si>
-    <t>O-ring, 10mm ID x 14mm OD x 2mmT</t>
-  </si>
-  <si>
-    <t>PRO-PF 32-249A</t>
-  </si>
-  <si>
-    <t>Spring Guide</t>
-  </si>
-  <si>
-    <t>BUI-MAT_1001</t>
-  </si>
-  <si>
-    <t>Plywood, Ordinary, 4.5mm x 8ft</t>
+    <t>CON-CON_1016</t>
+  </si>
+  <si>
+    <t>Scraper; Metal, 3"</t>
+  </si>
+  <si>
+    <t>CON-HOU_1006</t>
+  </si>
+  <si>
+    <t>Soap, liquid</t>
+  </si>
+  <si>
+    <t>CON-HOU_1004</t>
+  </si>
+  <si>
+    <t>Stretch Film, 20micron x 500mm x 500mtr</t>
+  </si>
+  <si>
+    <t>CON-HOU_1007</t>
+  </si>
+  <si>
+    <t>Stretch Film; 20 microns x 300mm x 150 meter</t>
+  </si>
+  <si>
+    <t>CON-OFF_1002</t>
+  </si>
+  <si>
+    <t>Tape, Masking 2"</t>
+  </si>
+  <si>
+    <t>PRO-PF 15-11/31 (B)</t>
+  </si>
+  <si>
+    <t>Upper Guide Bush (PF 15-11/31B)</t>
+  </si>
+  <si>
+    <t>PRO-PF 73-38</t>
+  </si>
+  <si>
+    <t>V Packing</t>
   </si>
   <si>
     <t>CON-CHE_1001</t>
@@ -95,16 +437,10 @@
     <t>Vappro 868 VCI Corrosion Inbitor Wax Coating (4 liters/gallon)</t>
   </si>
   <si>
-    <t>CON-FUE_1001</t>
-  </si>
-  <si>
-    <t>Diesel, Fuel-Save</t>
-  </si>
-  <si>
-    <t>CON-CON_1002</t>
-  </si>
-  <si>
-    <t>Paint Brush 1"</t>
+    <t>PRO-PF 73-39</t>
+  </si>
+  <si>
+    <t>Wire</t>
   </si>
 </sst>
 </file>
@@ -264,7 +600,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1152525" cy="333375"/>
+    <xdr:ext cx="1104900" cy="333375"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Sample image" descr="Sample image"/>
@@ -580,7 +916,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I2" sqref="I2"/>
@@ -701,7 +1037,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -723,7 +1059,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -745,7 +1081,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -767,7 +1103,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="L14" s="2"/>
     </row>
@@ -789,7 +1125,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -811,7 +1147,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L16" s="2"/>
     </row>
@@ -820,12 +1156,12 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -833,7 +1169,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L17" s="2"/>
     </row>
@@ -842,12 +1178,12 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -855,7 +1191,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="2">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L18" s="2"/>
     </row>
@@ -864,12 +1200,12 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -877,7 +1213,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L19" s="2"/>
     </row>
@@ -886,12 +1222,12 @@
         <v>10</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -899,7 +1235,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="2">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="L20" s="2"/>
     </row>
@@ -908,12 +1244,12 @@
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -921,22 +1257,1189 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="2">
+        <v>699</v>
+      </c>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="3">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2">
+        <v>3</v>
+      </c>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="3">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="3">
+        <v>14</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="2">
+        <v>5</v>
+      </c>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="3">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="2">
+        <v>17</v>
+      </c>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="3">
+        <v>16</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="3">
+        <v>17</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="3">
+        <v>18</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="3">
+        <v>19</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="3">
+        <v>20</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="3">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="3">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="3">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="3">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="3">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="2">
+        <v>314</v>
+      </c>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="3">
+        <v>26</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="2">
+        <v>148</v>
+      </c>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="3">
+        <v>27</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="2">
+        <v>22</v>
+      </c>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="3">
+        <v>28</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="2">
+        <v>19</v>
+      </c>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="3">
+        <v>29</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="2">
+        <v>21</v>
+      </c>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="3">
+        <v>30</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="2">
+        <v>95</v>
+      </c>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="3">
+        <v>31</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="2">
+        <v>447</v>
+      </c>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="3">
+        <v>32</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="2">
+        <v>26</v>
+      </c>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="3">
+        <v>33</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="2">
+        <v>246</v>
+      </c>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="3">
+        <v>34</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="2">
+        <v>111</v>
+      </c>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="3">
+        <v>35</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="2">
+        <v>150</v>
+      </c>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="3">
+        <v>36</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="2">
+        <v>227</v>
+      </c>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="3">
+        <v>37</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="2">
+        <v>297</v>
+      </c>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="3">
+        <v>38</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="2">
+        <v>8</v>
+      </c>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="3">
+        <v>39</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="2">
+        <v>240</v>
+      </c>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="3">
+        <v>40</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="2">
+        <v>200</v>
+      </c>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="3">
+        <v>41</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="2">
+        <v>52</v>
+      </c>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="3">
+        <v>42</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="2">
+        <v>52</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="3">
+        <v>43</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="2">
+        <v>102</v>
+      </c>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="3">
+        <v>44</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="2">
+        <v>91</v>
+      </c>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="3">
+        <v>45</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="2">
+        <v>82</v>
+      </c>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="3">
+        <v>46</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="2">
+        <v>2</v>
+      </c>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="3">
+        <v>47</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="2">
+        <v>7</v>
+      </c>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="3">
+        <v>48</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="2">
+        <v>8</v>
+      </c>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="3">
+        <v>49</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="2">
+        <v>8</v>
+      </c>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="3">
+        <v>50</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="2">
+        <v>10</v>
+      </c>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="3">
+        <v>51</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="2">
+        <v>0</v>
+      </c>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="3">
+        <v>52</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="2">
+        <v>6</v>
+      </c>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="3">
+        <v>53</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="2">
+        <v>1</v>
+      </c>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="3">
+        <v>54</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="2">
+        <v>85</v>
+      </c>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="3">
+        <v>55</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="2">
+        <v>0</v>
+      </c>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="3">
+        <v>56</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="2">
+        <v>2</v>
+      </c>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="3">
+        <v>57</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="2">
+        <v>0</v>
+      </c>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="3">
+        <v>58</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="2">
+        <v>2</v>
+      </c>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="3">
+        <v>59</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="2">
+        <v>2</v>
+      </c>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="3">
+        <v>60</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="2">
+        <v>5</v>
+      </c>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="3">
+        <v>61</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="2">
+        <v>96</v>
+      </c>
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="3">
+        <v>62</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="2">
+        <v>2</v>
+      </c>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="3">
+        <v>63</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="2">
+        <v>6</v>
+      </c>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="3">
+        <v>64</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="2">
+        <v>2</v>
+      </c>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -952,8 +2455,64 @@
     <protectedRange name="pc50f46460d60af4a12be7f76f62885a3" sqref="A19:L19" password="C724"/>
     <protectedRange name="p8bcd6afac17c7426eaa7f7963d983e9b" sqref="A20:L20" password="C724"/>
     <protectedRange name="pc919c27637143ab587e932d817f18adc" sqref="A21:L21" password="C724"/>
+    <protectedRange name="pb6e0bddd6ad21e18f86a495afee469bc" sqref="A22:L22" password="C724"/>
+    <protectedRange name="p2f11b84e241fcd2b18acb0eb3e94da7f" sqref="A23:L23" password="C724"/>
+    <protectedRange name="p4cb9c1e34bac19e1c5ea59ab0a283290" sqref="A24:L24" password="C724"/>
+    <protectedRange name="p04020568646ccb7aa32266f71af96a66" sqref="A25:L25" password="C724"/>
+    <protectedRange name="pcd58175ca5b5cbcd95d6217e063e3e74" sqref="A26:L26" password="C724"/>
+    <protectedRange name="pb8329879d2d4dd27170b88e397d6adff" sqref="A27:L27" password="C724"/>
+    <protectedRange name="p792eb50908d0b0b0855b399f2a8c0377" sqref="A28:L28" password="C724"/>
+    <protectedRange name="p122f56dae638dea3ab65427fa4e96e35" sqref="A29:L29" password="C724"/>
+    <protectedRange name="p0fb921e30017435bc98117ba8762e7b6" sqref="A30:L30" password="C724"/>
+    <protectedRange name="pb1be74cbb7d447e3fbbb0ec60e062a27" sqref="A31:L31" password="C724"/>
+    <protectedRange name="p330fd6088892a813da562aff13494024" sqref="A32:L32" password="C724"/>
+    <protectedRange name="pce386e1e5f6f5725867f97977d8cbbc9" sqref="A33:L33" password="C724"/>
+    <protectedRange name="p5e01b1b811f1ee2d39d4afd5d19fac24" sqref="A34:L34" password="C724"/>
+    <protectedRange name="p0a3d91b186c83d1a36ecb0d903a499bc" sqref="A35:L35" password="C724"/>
+    <protectedRange name="pbfacf7e548d02ffdef60fcf39f548a7f" sqref="A36:L36" password="C724"/>
+    <protectedRange name="p2295e593bfee1d3064118e35d721dff9" sqref="A37:L37" password="C724"/>
+    <protectedRange name="p7e9f7bc72ff22d9feaa274a551e6dbb7" sqref="A38:L38" password="C724"/>
+    <protectedRange name="p966ee030a845f6da648b5592aa19c0ae" sqref="A39:L39" password="C724"/>
+    <protectedRange name="p65a7e7116b4c6d6923b1953e552741b5" sqref="A40:L40" password="C724"/>
+    <protectedRange name="p910355017052919470dbb33cc9983253" sqref="A41:L41" password="C724"/>
+    <protectedRange name="p0396d89e85d888449f06336c6e1924b2" sqref="A42:L42" password="C724"/>
+    <protectedRange name="p4191caa6c6c0654eb3c50e40cfad14b6" sqref="A43:L43" password="C724"/>
+    <protectedRange name="p3cc308ca08bd254b126133b27678b275" sqref="A44:L44" password="C724"/>
+    <protectedRange name="p9a1fb295366aefd7df9215a4b1887a7a" sqref="A45:L45" password="C724"/>
+    <protectedRange name="p9a90c916bc18c23a188858f3f18ab149" sqref="A46:L46" password="C724"/>
+    <protectedRange name="p112f4b5ef694d38053716354bba123db" sqref="A47:L47" password="C724"/>
+    <protectedRange name="pe6c023c22e4a9b9bf2e062b1cedc9667" sqref="A48:L48" password="C724"/>
+    <protectedRange name="p01035cd26e61fc7785cebc4d47106544" sqref="A49:L49" password="C724"/>
+    <protectedRange name="p728aeb07059df39b6c3dff123e529e65" sqref="A50:L50" password="C724"/>
+    <protectedRange name="pfd3a0c01da62f37992ef47d800276136" sqref="A51:L51" password="C724"/>
+    <protectedRange name="p83a352003dd608527d755d216a907ea9" sqref="A52:L52" password="C724"/>
+    <protectedRange name="p83605c2b793db76e30a9c3525e7c5647" sqref="A53:L53" password="C724"/>
+    <protectedRange name="pab373d9c573bcdb48fe6bf01349b4ed0" sqref="A54:L54" password="C724"/>
+    <protectedRange name="p9da80a0d163a20690b332facfa60d5de" sqref="A55:L55" password="C724"/>
+    <protectedRange name="p3d183ce75135f0d3a34504ca48f6cf60" sqref="A56:L56" password="C724"/>
+    <protectedRange name="p0a1e9647ad3fbad1e1d1f8f69724f726" sqref="A57:L57" password="C724"/>
+    <protectedRange name="pd3f0d6d11ce6a69ff843707977505a0c" sqref="A58:L58" password="C724"/>
+    <protectedRange name="p9a6888be5b0f6f941f5bc8b0c9b5f164" sqref="A59:L59" password="C724"/>
+    <protectedRange name="pff7719fa29945d00fe0dc2c3cee7149e" sqref="A60:L60" password="C724"/>
+    <protectedRange name="p6164ac62d75351cbf6e049698c406b40" sqref="A61:L61" password="C724"/>
+    <protectedRange name="pd59ba13c14c079649343eca560fa0c20" sqref="A62:L62" password="C724"/>
+    <protectedRange name="p102c53ad6a1af1309fdded31eea543f1" sqref="A63:L63" password="C724"/>
+    <protectedRange name="p283064956e76d2227c627fa40041093b" sqref="A64:L64" password="C724"/>
+    <protectedRange name="p88062467387924d5d5e7cebcabfa6a97" sqref="A65:L65" password="C724"/>
+    <protectedRange name="p76e304b3b58823e5217f5d01944d1e1f" sqref="A66:L66" password="C724"/>
+    <protectedRange name="p03479c94f9b5ecdddf0604e9a16004ce" sqref="A67:L67" password="C724"/>
+    <protectedRange name="pbc146b288590c4976f2763d7cf453525" sqref="A68:L68" password="C724"/>
+    <protectedRange name="pd0843e31ab28b2cab68ddb443c9e4964" sqref="A69:L69" password="C724"/>
+    <protectedRange name="p459ee7cff63992c05e753f6ece273afb" sqref="A70:L70" password="C724"/>
+    <protectedRange name="p797ff8ae36ea6c8b5d60a941e180193f" sqref="A71:L71" password="C724"/>
+    <protectedRange name="pef3ebe34c34d59fc6fcdbe235836f184" sqref="A72:L72" password="C724"/>
+    <protectedRange name="pfa202b2436f48749fa819cf210c4f89f" sqref="A73:L73" password="C724"/>
+    <protectedRange name="p5b8d927580bdcfab70c279b5eaf343c6" sqref="A74:L74" password="C724"/>
   </protectedRanges>
   <mergeCells>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="K11:L11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="K12:L12"/>
@@ -987,12 +2546,165 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="K22:L22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E49:J49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:J56"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="E58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="E59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:J60"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="E61:J61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:J62"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:J63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:J65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="E66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:J67"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:J68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="E69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="E70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="E71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="E72:J72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="E73:J73"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="E74:J74"/>
+    <mergeCell ref="K74:L74"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:J10"/>
     <mergeCell ref="K10:L10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="K11:L11"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="I2:K2"/>
   </mergeCells>

</xml_diff>

<commit_message>
FROM - TO   receive issue report
</commit_message>
<xml_diff>
--- a/Inventory Report.xlsx
+++ b/Inventory Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
   <si>
     <t>PROGEN Dieseltech Services Corp.</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Purok San Jose, Brgy. Calumangan, Bago City</t>
   </si>
   <si>
-    <t>AS OF June 24, 2020</t>
+    <t>AS OF July 5, 2021</t>
   </si>
   <si>
     <t>Negros Occidental, Philippines 6101</t>
@@ -38,7 +38,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2020-03-31 - 2020-06-24</t>
+    <t>2020-11-07 - 2021-07-05</t>
   </si>
   <si>
     <t>Warehouse</t>
@@ -68,22 +68,394 @@
     <t>"Express" Union</t>
   </si>
   <si>
+    <t>K 27046 B</t>
+  </si>
+  <si>
+    <t>(BIG) Tubular Sealing for Cover K 27007 and Bearing Casing K 28001</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1056</t>
+  </si>
+  <si>
+    <t>3 way Valve w/o Bolt</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1057</t>
+  </si>
+  <si>
+    <t>3 way Valve, Complete</t>
+  </si>
+  <si>
+    <t>K 47034</t>
+  </si>
+  <si>
+    <t>3-way Valve, Complete</t>
+  </si>
+  <si>
+    <t>CON-CHE_1011</t>
+  </si>
+  <si>
+    <t>Acetylene</t>
+  </si>
+  <si>
+    <t>CON-EIC_1004</t>
+  </si>
+  <si>
+    <t>Aluminum Foil, FSK 7150 A, 3 way Reinforced, with scrim craft paper packing. Size: 1.25m (W) x 120m (L)</t>
+  </si>
+  <si>
+    <t>CON-CON_1037</t>
+  </si>
+  <si>
+    <t>Bag; Garbage, Size: XXL, (1 roll = 10 pcs.)</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1082</t>
+  </si>
+  <si>
+    <t>Ball Bearing, 5206</t>
+  </si>
+  <si>
+    <t>CON-EIC_1003</t>
+  </si>
+  <si>
+    <t>Battery, AAA</t>
+  </si>
+  <si>
+    <t>CON-CON_1008</t>
+  </si>
+  <si>
+    <t>Blade; Hacksaw, 18 TPI</t>
+  </si>
+  <si>
+    <t>CON-CON_1004</t>
+  </si>
+  <si>
+    <t>Brush, Paint, 2"</t>
+  </si>
+  <si>
+    <t>CON-CON_1005</t>
+  </si>
+  <si>
+    <t>Brush, Steel</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1085</t>
+  </si>
+  <si>
+    <t>Bush, WE-17168</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1088</t>
+  </si>
+  <si>
+    <t>Cambire Tubing, 1 1/6x1mm, ISL-09/E</t>
+  </si>
+  <si>
+    <t>FFE-OFF_1002</t>
+  </si>
+  <si>
+    <t>Cash Box, 6" w/key and number combination</t>
+  </si>
+  <si>
+    <t>TOO-POW_1002</t>
+  </si>
+  <si>
+    <t>Cutter, Grass, Brand: Makita Model: EBH34OU, serial#: EH035A174170135Y</t>
+  </si>
+  <si>
+    <t>CON-FUE_1003</t>
+  </si>
+  <si>
+    <t>Diesel Engine Oil HD, API CF/SF, SAE 40, Mono Grade, Rev-X</t>
+  </si>
+  <si>
     <t>CON-FUE_1001</t>
   </si>
   <si>
     <t>Diesel, Fuel-Save</t>
   </si>
   <si>
-    <t>EIC-PAR_1001</t>
-  </si>
-  <si>
-    <t>Potential Transformer, Part Number: PTW4-2-75-722FF, Part ID: 109562</t>
+    <t>CON-CON_1041</t>
+  </si>
+  <si>
+    <t>Electrode, Welding, 1/8" x 12", E6011</t>
+  </si>
+  <si>
+    <t>K 81138</t>
+  </si>
+  <si>
+    <t>Expansion Bellows for Exhaust Piping, 10 Corrugations</t>
+  </si>
+  <si>
+    <t>K 81137</t>
+  </si>
+  <si>
+    <t>Expansion Bellows, 6 Corrogations</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1084</t>
+  </si>
+  <si>
+    <t>Fabrication Ring, 73x88x4mm</t>
+  </si>
+  <si>
+    <t>CON-CON_1052</t>
+  </si>
+  <si>
+    <t>Foam, 2" thick, 36" width, 75" length, brand: PU2 Uratex</t>
+  </si>
+  <si>
+    <t>FFE-PPE_1002</t>
+  </si>
+  <si>
+    <t>Gloves, Chemical Resistance, Nitrile with Cotton Flock Lining, Large</t>
+  </si>
+  <si>
+    <t>CON-HOU_1003</t>
+  </si>
+  <si>
+    <t>Gloves, Cotton</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1044</t>
+  </si>
+  <si>
+    <t>High Heat Packing, 2.6 m</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1045</t>
+  </si>
+  <si>
+    <t>High Heat Packing, 4.8</t>
+  </si>
+  <si>
+    <t>CON-FUE_1004</t>
+  </si>
+  <si>
+    <t>Kerosene</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1294</t>
+  </si>
+  <si>
+    <t>Key, SJ6-G9</t>
+  </si>
+  <si>
+    <t>CON-CON_1043</t>
+  </si>
+  <si>
+    <t>Lumber; Good, 2" x 2" x 10 ft, Mahogany</t>
+  </si>
+  <si>
+    <t>CON-CON_1013</t>
+  </si>
+  <si>
+    <t>Lumber; Good, 2" x 3" x 10 ft, Mahogany</t>
+  </si>
+  <si>
+    <t>CON-OFF_1001</t>
+  </si>
+  <si>
+    <t>Marker, Metal, Color: Yellow</t>
+  </si>
+  <si>
+    <t>CON-CON_1021</t>
+  </si>
+  <si>
+    <t>Metal Polish, Premium Grade, 150ml</t>
+  </si>
+  <si>
+    <t>CON-CON_1042</t>
+  </si>
+  <si>
+    <t>Nails, Common, 2"</t>
+  </si>
+  <si>
+    <t>CON-CON_1010</t>
+  </si>
+  <si>
+    <t>Nails, Common, 3"</t>
+  </si>
+  <si>
+    <t>CON-CON_1009</t>
+  </si>
+  <si>
+    <t>Nails, Common, 4"</t>
+  </si>
+  <si>
+    <t>CON-CON_1012</t>
+  </si>
+  <si>
+    <t>Nails; Common, 1 1/2"</t>
+  </si>
+  <si>
+    <t>CON-CHE_1010</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1083</t>
+  </si>
+  <si>
+    <t>Packing, SJ-3052002</t>
+  </si>
+  <si>
+    <t>CON-CON_1034</t>
+  </si>
+  <si>
+    <t>Paint, Enamel, Uni Apple Green, 4L = 1Gal</t>
+  </si>
+  <si>
+    <t>CON-CON_1051</t>
+  </si>
+  <si>
+    <t>Paint, Latex, Apple Green, 4L = 1Gal</t>
+  </si>
+  <si>
+    <t>CON-CON_1007</t>
+  </si>
+  <si>
+    <t>Paint, Primer, Epoxy, Gray, With Catalyst, 4L/gal</t>
+  </si>
+  <si>
+    <t>CON-CON_1040</t>
+  </si>
+  <si>
+    <t>Paint, Remover</t>
+  </si>
+  <si>
+    <t>CON-CON_1017</t>
+  </si>
+  <si>
+    <t>Plywood, Ordinary, 4ft x 8ft x 5mm</t>
+  </si>
+  <si>
+    <t>EIC-PAR_1179</t>
+  </si>
+  <si>
+    <t>Potentiometer, Motorized, Brand: Selco, 1 turn, E7800-0640/E7800-23-00, 24Vdc, 5k ohms, 2Watts, 0.8-6.0 rpm</t>
   </si>
   <si>
     <t>CON-HOU_1001</t>
   </si>
   <si>
     <t>Rags, Cotton</t>
+  </si>
+  <si>
+    <t>K 81150</t>
+  </si>
+  <si>
+    <t>Ring, Two Part for Exhaust Piping, K81150</t>
+  </si>
+  <si>
+    <t>K 81140</t>
+  </si>
+  <si>
+    <t>Ring, Two Part, for Exhaust Piping, K81140</t>
+  </si>
+  <si>
+    <t>K 81145</t>
+  </si>
+  <si>
+    <t>Ring, Two Parts for Compensator, K81145</t>
+  </si>
+  <si>
+    <t>CON-CON_1003</t>
+  </si>
+  <si>
+    <t>Sand Paper, G120</t>
+  </si>
+  <si>
+    <t>CON-CON_1046</t>
+  </si>
+  <si>
+    <t>Sand Paper, G150</t>
+  </si>
+  <si>
+    <t>CON-CON_1001</t>
+  </si>
+  <si>
+    <t>Scraper, Industrial; Size: 2"</t>
+  </si>
+  <si>
+    <t>CON-HOU_1006</t>
+  </si>
+  <si>
+    <t>Soap, liquid</t>
+  </si>
+  <si>
+    <t>CON-CHE_1015</t>
+  </si>
+  <si>
+    <t>Solignum, Wood Preservatives, Color Brown</t>
+  </si>
+  <si>
+    <t>AUX-PAR_1089</t>
+  </si>
+  <si>
+    <t>Spring Collar_Aux</t>
+  </si>
+  <si>
+    <t>FFE-OFF_1001</t>
+  </si>
+  <si>
+    <t>Stand Fan, 16", Brand: Union</t>
+  </si>
+  <si>
+    <t>CON-HOU_1007</t>
+  </si>
+  <si>
+    <t>Stretch Film; 20 microns x 300mm x 150 meter</t>
+  </si>
+  <si>
+    <t>CON-OFF_1005</t>
+  </si>
+  <si>
+    <t>Tape, Masking 1"</t>
+  </si>
+  <si>
+    <t>CON-OFF_1002</t>
+  </si>
+  <si>
+    <t>Tape, Masking 2"</t>
+  </si>
+  <si>
+    <t>FFE-SSE_1003</t>
+  </si>
+  <si>
+    <t>Tarpaulin; (Yellow-Green, Heavy Duty), 44 ft. x 36 ft.,</t>
+  </si>
+  <si>
+    <t>FFE-TES_1001</t>
+  </si>
+  <si>
+    <t>Thickness Meter, Ultrasonic, Model: TM-8812</t>
+  </si>
+  <si>
+    <t>CON-CON_1019</t>
+  </si>
+  <si>
+    <t>Thinner; Lacquer</t>
+  </si>
+  <si>
+    <t>CON-CON_1045</t>
+  </si>
+  <si>
+    <t>Top Coat, Enamel type, Solid Varnish Clear</t>
+  </si>
+  <si>
+    <t>FFE-OFF_1003</t>
+  </si>
+  <si>
+    <t>UPS, Vertiv Liebert ITON-SOHO, PSA650-SOHO, SN#: 241907400977SH</t>
+  </si>
+  <si>
+    <t>CON-CON_1050</t>
+  </si>
+  <si>
+    <t>Wheel, Grinding for Bench Grinder, 6" x 1/2" x 1"</t>
   </si>
 </sst>
 </file>
@@ -559,7 +931,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I2" sqref="I2"/>
@@ -686,7 +1058,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -708,7 +1080,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="2">
-        <v>20</v>
+        <v>209</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -730,7 +1102,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -752,9 +1124,1373 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2">
+        <v>12</v>
+      </c>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="2">
+        <v>20</v>
+      </c>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="3">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="3">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2">
+        <v>40</v>
+      </c>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="3">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="3">
         <v>10</v>
       </c>
-      <c r="L14" s="2"/>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="3">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="2">
+        <v>5</v>
+      </c>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="3">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2">
+        <v>7</v>
+      </c>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="3">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="2">
+        <v>12</v>
+      </c>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="3">
+        <v>14</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="2">
+        <v>13</v>
+      </c>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="3">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="2">
+        <v>10</v>
+      </c>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="3">
+        <v>16</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="3">
+        <v>17</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="3">
+        <v>18</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="2">
+        <v>2</v>
+      </c>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="3">
+        <v>19</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="2">
+        <v>50</v>
+      </c>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="3">
+        <v>20</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2">
+        <v>5</v>
+      </c>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="3">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2">
+        <v>6</v>
+      </c>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="3">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="2">
+        <v>12</v>
+      </c>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="3">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="2">
+        <v>2</v>
+      </c>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="3">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="2">
+        <v>1</v>
+      </c>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="3">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="2">
+        <v>6</v>
+      </c>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="3">
+        <v>26</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="3">
+        <v>27</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="3">
+        <v>28</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="3">
+        <v>29</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="3">
+        <v>30</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="2">
+        <v>65</v>
+      </c>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="3">
+        <v>31</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="2">
+        <v>43</v>
+      </c>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="3">
+        <v>32</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="2">
+        <v>22</v>
+      </c>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="3">
+        <v>33</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="2">
+        <v>3</v>
+      </c>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="3">
+        <v>34</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="2">
+        <v>2</v>
+      </c>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="3">
+        <v>35</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="2">
+        <v>9</v>
+      </c>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="3">
+        <v>36</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="2">
+        <v>13</v>
+      </c>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="3">
+        <v>37</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="2">
+        <v>10</v>
+      </c>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="3">
+        <v>38</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="2">
+        <v>14</v>
+      </c>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="3">
+        <v>39</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="2">
+        <v>2</v>
+      </c>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="3">
+        <v>40</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="2">
+        <v>2</v>
+      </c>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="3">
+        <v>41</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="2">
+        <v>4</v>
+      </c>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="3">
+        <v>42</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="2">
+        <v>1</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="3">
+        <v>43</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="2">
+        <v>5</v>
+      </c>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="3">
+        <v>44</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="2">
+        <v>2</v>
+      </c>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="3">
+        <v>45</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="2">
+        <v>21</v>
+      </c>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="3">
+        <v>46</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="2">
+        <v>1</v>
+      </c>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="3">
+        <v>47</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="2">
+        <v>37.5</v>
+      </c>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="3">
+        <v>48</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="2">
+        <v>12</v>
+      </c>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="3">
+        <v>49</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="2">
+        <v>12</v>
+      </c>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="3">
+        <v>50</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="2">
+        <v>12</v>
+      </c>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="3">
+        <v>51</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="2">
+        <v>127</v>
+      </c>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="3">
+        <v>52</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="2">
+        <v>42</v>
+      </c>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="3">
+        <v>53</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="2">
+        <v>5</v>
+      </c>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="3">
+        <v>54</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="2">
+        <v>3</v>
+      </c>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="3">
+        <v>55</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="2">
+        <v>1</v>
+      </c>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="3">
+        <v>56</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="2">
+        <v>50</v>
+      </c>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="3">
+        <v>57</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="2">
+        <v>0</v>
+      </c>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="3">
+        <v>58</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="2">
+        <v>1</v>
+      </c>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="3">
+        <v>59</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="2">
+        <v>8</v>
+      </c>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="3">
+        <v>60</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="2">
+        <v>18</v>
+      </c>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="3">
+        <v>61</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="2">
+        <v>0</v>
+      </c>
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="3">
+        <v>62</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="2">
+        <v>1</v>
+      </c>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="3">
+        <v>63</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="2">
+        <v>4</v>
+      </c>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="3">
+        <v>64</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="2">
+        <v>3</v>
+      </c>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="3">
+        <v>65</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="2">
+        <v>1</v>
+      </c>
+      <c r="L75" s="2"/>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="3">
+        <v>66</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="2">
+        <v>4</v>
+      </c>
+      <c r="L76" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -763,6 +2499,68 @@
     <protectedRange name="p647420430d97ec1d7412055efbe73ee6" sqref="A12:L12" password="C724"/>
     <protectedRange name="pb1d1f8d24dd55af59a30420f29198236" sqref="A13:L13" password="C724"/>
     <protectedRange name="p488e11d98b179631bf2547f4444243a4" sqref="A14:L14" password="C724"/>
+    <protectedRange name="pf6b0e90628197f4a0b92055cdd5ea018" sqref="A15:L15" password="C724"/>
+    <protectedRange name="p2b7b85a6053707c007a3bc2217c3e7d9" sqref="A16:L16" password="C724"/>
+    <protectedRange name="pb4cbcb6d7a30f244bc0b089328b79204" sqref="A17:L17" password="C724"/>
+    <protectedRange name="p1683364c499bbb2b53cf65cee8471773" sqref="A18:L18" password="C724"/>
+    <protectedRange name="pc50f46460d60af4a12be7f76f62885a3" sqref="A19:L19" password="C724"/>
+    <protectedRange name="p8bcd6afac17c7426eaa7f7963d983e9b" sqref="A20:L20" password="C724"/>
+    <protectedRange name="pc919c27637143ab587e932d817f18adc" sqref="A21:L21" password="C724"/>
+    <protectedRange name="pb6e0bddd6ad21e18f86a495afee469bc" sqref="A22:L22" password="C724"/>
+    <protectedRange name="p2f11b84e241fcd2b18acb0eb3e94da7f" sqref="A23:L23" password="C724"/>
+    <protectedRange name="p4cb9c1e34bac19e1c5ea59ab0a283290" sqref="A24:L24" password="C724"/>
+    <protectedRange name="p04020568646ccb7aa32266f71af96a66" sqref="A25:L25" password="C724"/>
+    <protectedRange name="pcd58175ca5b5cbcd95d6217e063e3e74" sqref="A26:L26" password="C724"/>
+    <protectedRange name="pb8329879d2d4dd27170b88e397d6adff" sqref="A27:L27" password="C724"/>
+    <protectedRange name="p792eb50908d0b0b0855b399f2a8c0377" sqref="A28:L28" password="C724"/>
+    <protectedRange name="p122f56dae638dea3ab65427fa4e96e35" sqref="A29:L29" password="C724"/>
+    <protectedRange name="p0fb921e30017435bc98117ba8762e7b6" sqref="A30:L30" password="C724"/>
+    <protectedRange name="pb1be74cbb7d447e3fbbb0ec60e062a27" sqref="A31:L31" password="C724"/>
+    <protectedRange name="p330fd6088892a813da562aff13494024" sqref="A32:L32" password="C724"/>
+    <protectedRange name="pce386e1e5f6f5725867f97977d8cbbc9" sqref="A33:L33" password="C724"/>
+    <protectedRange name="p5e01b1b811f1ee2d39d4afd5d19fac24" sqref="A34:L34" password="C724"/>
+    <protectedRange name="p0a3d91b186c83d1a36ecb0d903a499bc" sqref="A35:L35" password="C724"/>
+    <protectedRange name="pbfacf7e548d02ffdef60fcf39f548a7f" sqref="A36:L36" password="C724"/>
+    <protectedRange name="p2295e593bfee1d3064118e35d721dff9" sqref="A37:L37" password="C724"/>
+    <protectedRange name="p7e9f7bc72ff22d9feaa274a551e6dbb7" sqref="A38:L38" password="C724"/>
+    <protectedRange name="p966ee030a845f6da648b5592aa19c0ae" sqref="A39:L39" password="C724"/>
+    <protectedRange name="p65a7e7116b4c6d6923b1953e552741b5" sqref="A40:L40" password="C724"/>
+    <protectedRange name="p910355017052919470dbb33cc9983253" sqref="A41:L41" password="C724"/>
+    <protectedRange name="p0396d89e85d888449f06336c6e1924b2" sqref="A42:L42" password="C724"/>
+    <protectedRange name="p4191caa6c6c0654eb3c50e40cfad14b6" sqref="A43:L43" password="C724"/>
+    <protectedRange name="p3cc308ca08bd254b126133b27678b275" sqref="A44:L44" password="C724"/>
+    <protectedRange name="p9a1fb295366aefd7df9215a4b1887a7a" sqref="A45:L45" password="C724"/>
+    <protectedRange name="p9a90c916bc18c23a188858f3f18ab149" sqref="A46:L46" password="C724"/>
+    <protectedRange name="p112f4b5ef694d38053716354bba123db" sqref="A47:L47" password="C724"/>
+    <protectedRange name="pe6c023c22e4a9b9bf2e062b1cedc9667" sqref="A48:L48" password="C724"/>
+    <protectedRange name="p01035cd26e61fc7785cebc4d47106544" sqref="A49:L49" password="C724"/>
+    <protectedRange name="p728aeb07059df39b6c3dff123e529e65" sqref="A50:L50" password="C724"/>
+    <protectedRange name="pfd3a0c01da62f37992ef47d800276136" sqref="A51:L51" password="C724"/>
+    <protectedRange name="p83a352003dd608527d755d216a907ea9" sqref="A52:L52" password="C724"/>
+    <protectedRange name="p83605c2b793db76e30a9c3525e7c5647" sqref="A53:L53" password="C724"/>
+    <protectedRange name="pab373d9c573bcdb48fe6bf01349b4ed0" sqref="A54:L54" password="C724"/>
+    <protectedRange name="p9da80a0d163a20690b332facfa60d5de" sqref="A55:L55" password="C724"/>
+    <protectedRange name="p3d183ce75135f0d3a34504ca48f6cf60" sqref="A56:L56" password="C724"/>
+    <protectedRange name="p0a1e9647ad3fbad1e1d1f8f69724f726" sqref="A57:L57" password="C724"/>
+    <protectedRange name="pd3f0d6d11ce6a69ff843707977505a0c" sqref="A58:L58" password="C724"/>
+    <protectedRange name="p9a6888be5b0f6f941f5bc8b0c9b5f164" sqref="A59:L59" password="C724"/>
+    <protectedRange name="pff7719fa29945d00fe0dc2c3cee7149e" sqref="A60:L60" password="C724"/>
+    <protectedRange name="p6164ac62d75351cbf6e049698c406b40" sqref="A61:L61" password="C724"/>
+    <protectedRange name="pd59ba13c14c079649343eca560fa0c20" sqref="A62:L62" password="C724"/>
+    <protectedRange name="p102c53ad6a1af1309fdded31eea543f1" sqref="A63:L63" password="C724"/>
+    <protectedRange name="p283064956e76d2227c627fa40041093b" sqref="A64:L64" password="C724"/>
+    <protectedRange name="p88062467387924d5d5e7cebcabfa6a97" sqref="A65:L65" password="C724"/>
+    <protectedRange name="p76e304b3b58823e5217f5d01944d1e1f" sqref="A66:L66" password="C724"/>
+    <protectedRange name="p03479c94f9b5ecdddf0604e9a16004ce" sqref="A67:L67" password="C724"/>
+    <protectedRange name="pbc146b288590c4976f2763d7cf453525" sqref="A68:L68" password="C724"/>
+    <protectedRange name="pd0843e31ab28b2cab68ddb443c9e4964" sqref="A69:L69" password="C724"/>
+    <protectedRange name="p459ee7cff63992c05e753f6ece273afb" sqref="A70:L70" password="C724"/>
+    <protectedRange name="p797ff8ae36ea6c8b5d60a941e180193f" sqref="A71:L71" password="C724"/>
+    <protectedRange name="pef3ebe34c34d59fc6fcdbe235836f184" sqref="A72:L72" password="C724"/>
+    <protectedRange name="pfa202b2436f48749fa819cf210c4f89f" sqref="A73:L73" password="C724"/>
+    <protectedRange name="p5b8d927580bdcfab70c279b5eaf343c6" sqref="A74:L74" password="C724"/>
+    <protectedRange name="p124a23cb1675e35b731db8e0548c2ed9" sqref="A75:L75" password="C724"/>
+    <protectedRange name="pa6a04e498f546ff8571ca7b735312318" sqref="A76:L76" password="C724"/>
   </protectedRanges>
   <mergeCells>
     <mergeCell ref="B11:D11"/>
@@ -777,6 +2575,192 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="K14:L14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E49:J49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:J56"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="E58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="E59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:J60"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="E61:J61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:J62"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:J63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:J65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="E66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:J67"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:J68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="E69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="E70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="E71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="E72:J72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="E73:J73"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="E74:J74"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="E75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="E76:J76"/>
+    <mergeCell ref="K76:L76"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:J10"/>
     <mergeCell ref="K10:L10"/>

</xml_diff>